<commit_message>
- Mejorando sistema de archivos - Trabajo con Excels - Mensaje para usuarios nuevos
</commit_message>
<xml_diff>
--- a/files/alumnos/dni_alumnos.xlsx
+++ b/files/alumnos/dni_alumnos.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chatbot_santa_lucia\files\identidades\secundaria\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\chatbot_santa_lucia\files\alumnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC8AF8-DA79-4D07-BE0B-9F45EAF446FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F078B3-37B9-4C59-BC75-A0F36A9CE361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-1155" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1a" sheetId="1" r:id="rId1"/>
+    <sheet name="dni_alumnos" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +22,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>secundaria</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,9 +72,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,26 +353,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B36F564-0175-460B-9BC5-E6FF45226F9E}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>41550112</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>11111111</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>21903130</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>22222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>33333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>